<commit_message>
Making sure the data input is equal to the base case
</commit_message>
<xml_diff>
--- a/AssignmentV2/Data/Generators_New.xlsx
+++ b/AssignmentV2/Data/Generators_New.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pablo Gutierrez\Desktop\Optimization in Modern Power Systems\Assignment\Opti\AssignmentV2\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leonr\OneDrive\Documents\DTU\OptimizationInPS\ProjectGit\Opti\AssignmentV2\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{836B9CD1-7397-468B-B83C-8B59D8B56B0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CFA5A0B-BA4A-46CE-93A6-2CE2652E7A2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{37D0B2D4-FDF1-45BA-8446-61EA4494B4A2}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" activeTab="2" xr2:uid="{37D0B2D4-FDF1-45BA-8446-61EA4494B4A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Generators_New" sheetId="1" r:id="rId1"/>
@@ -968,17 +968,17 @@
       <selection activeCell="D2" sqref="D2:D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="4" max="4" width="13.21875" customWidth="1"/>
+    <col min="4" max="4" width="13.19921875" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
     <col min="6" max="6" width="11.6640625" customWidth="1"/>
-    <col min="7" max="7" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.88671875" customWidth="1"/>
+    <col min="7" max="7" width="14.86328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.86328125" customWidth="1"/>
     <col min="9" max="9" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1010,7 +1010,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1042,7 +1042,7 @@
         <v>0.98599999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1074,7 +1074,7 @@
         <v>0.98599999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1106,7 +1106,7 @@
         <v>0.98599999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1138,7 +1138,7 @@
         <v>0.42899999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1170,7 +1170,7 @@
         <v>0.98599999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1202,7 +1202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1234,7 +1234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1266,7 +1266,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1298,7 +1298,7 @@
         <v>0.42899999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1330,7 +1330,7 @@
         <v>0.98599999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1362,7 +1362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1394,7 +1394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1426,7 +1426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1458,7 +1458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1490,7 +1490,7 @@
         <v>0.42899999999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1522,7 +1522,7 @@
         <v>0.98599999999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
         <v>0</v>
       </c>
@@ -1575,7 +1575,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
         <v>1</v>
       </c>
@@ -1653,13 +1653,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FDEA3BA-FF72-BE4E-99F7-358C6FECE33C}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -1667,7 +1667,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1675,7 +1675,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -1683,7 +1683,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -1691,20 +1691,20 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="1">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1716,20 +1716,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{781F5A14-CD09-4D7D-B01E-8FDF2EB93508}">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="2" max="2" width="11" customWidth="1"/>
-    <col min="3" max="3" width="11.44140625" customWidth="1"/>
-    <col min="5" max="5" width="16.109375" customWidth="1"/>
+    <col min="3" max="3" width="11.46484375" customWidth="1"/>
+    <col min="5" max="5" width="16.1328125" customWidth="1"/>
     <col min="6" max="6" width="12" customWidth="1"/>
     <col min="12" max="12" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1749,7 +1749,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1775,7 +1775,7 @@
       </c>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1801,7 +1801,7 @@
       </c>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1827,7 +1827,7 @@
       </c>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1853,7 +1853,7 @@
       </c>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1879,7 +1879,7 @@
       </c>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1893,7 +1893,7 @@
       </c>
       <c r="D7">
         <f>INDEX(Fuel_Cost_Absolute!$B$2:$B$6,MATCH( Python_Gen_N_Data!B7,Fuel_Cost_Absolute!$A$2:$A$6,0))</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E7">
         <f>Generators_New!G7</f>
@@ -1905,7 +1905,7 @@
       </c>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1919,7 +1919,7 @@
       </c>
       <c r="D8">
         <f>INDEX(Fuel_Cost_Absolute!$B$2:$B$6,MATCH( Python_Gen_N_Data!B8,Fuel_Cost_Absolute!$A$2:$A$6,0))</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E8">
         <f>Generators_New!G8</f>
@@ -1931,7 +1931,7 @@
       </c>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1945,7 +1945,7 @@
       </c>
       <c r="D9">
         <f>INDEX(Fuel_Cost_Absolute!$B$2:$B$6,MATCH( Python_Gen_N_Data!B9,Fuel_Cost_Absolute!$A$2:$A$6,0))</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E9">
         <f>Generators_New!G9</f>
@@ -1957,7 +1957,7 @@
       </c>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1983,7 +1983,7 @@
       </c>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>9</v>
       </c>
@@ -2009,7 +2009,7 @@
       </c>
       <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>10</v>
       </c>
@@ -2023,7 +2023,7 @@
       </c>
       <c r="D12">
         <f>INDEX(Fuel_Cost_Absolute!$B$2:$B$6,MATCH( Python_Gen_N_Data!B12,Fuel_Cost_Absolute!$A$2:$A$6,0))</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E12">
         <f>Generators_New!G12</f>
@@ -2035,7 +2035,7 @@
       </c>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>11</v>
       </c>
@@ -2049,7 +2049,7 @@
       </c>
       <c r="D13">
         <f>INDEX(Fuel_Cost_Absolute!$B$2:$B$6,MATCH( Python_Gen_N_Data!B13,Fuel_Cost_Absolute!$A$2:$A$6,0))</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E13">
         <f>Generators_New!G13</f>
@@ -2061,7 +2061,7 @@
       </c>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>12</v>
       </c>
@@ -2075,7 +2075,7 @@
       </c>
       <c r="D14">
         <f>INDEX(Fuel_Cost_Absolute!$B$2:$B$6,MATCH( Python_Gen_N_Data!B14,Fuel_Cost_Absolute!$A$2:$A$6,0))</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E14">
         <f>Generators_New!G14</f>
@@ -2087,7 +2087,7 @@
       </c>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>13</v>
       </c>
@@ -2101,7 +2101,7 @@
       </c>
       <c r="D15">
         <f>INDEX(Fuel_Cost_Absolute!$B$2:$B$6,MATCH( Python_Gen_N_Data!B15,Fuel_Cost_Absolute!$A$2:$A$6,0))</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E15">
         <f>Generators_New!G15</f>
@@ -2113,7 +2113,7 @@
       </c>
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>14</v>
       </c>
@@ -2139,7 +2139,7 @@
       </c>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>15</v>
       </c>
@@ -2178,9 +2178,9 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.53125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A1">
         <v>1</v>
       </c>
@@ -2230,7 +2230,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A2">
         <f>IF(Generators_New!B$22=0,1,0)</f>
         <v>1</v>
@@ -2296,7 +2296,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A3">
         <f>IF(Generators_New!B$22=1,1,0)</f>
         <v>0</v>

</xml_diff>